<commit_message>
Volcker Rule, SCCL, Dodd Frank, Capital Rules
Volcker Rule, SCCL, Dodd Frank, Capital Rules etc.
</commit_message>
<xml_diff>
--- a/SCCL_Volcker_DoddFrank_MarketCapitalRule.xlsx
+++ b/SCCL_Volcker_DoddFrank_MarketCapitalRule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jobs_2021_2022\GITHUB-Upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacka\OneDrive\Desktop\GITHUB_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07B5B05-8168-418F-977C-B8FEA775077A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE4EDA-A4FD-4BB1-8FA8-401FD7166635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="655" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="655" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCCL" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="CFTC_Capital_Rule" sheetId="7" r:id="rId6"/>
     <sheet name="SR 11-07" sheetId="6" r:id="rId7"/>
     <sheet name="SR 11-10" sheetId="8" r:id="rId8"/>
-    <sheet name="IRRBB" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Net exposure is measured against the bank’s tier 1 capital - 5% of tier 1 capital.</t>
   </si>
@@ -659,15 +658,6 @@
   </si>
   <si>
     <t xml:space="preserve">CCR is a multidimensional form of risk, affected by both the exposure to a counterparty and the credit quality of the counterparty, both of which are sensitive to market-induced changes. It is also affected by the interaction of these risks, for example the correlation  between an exposure and the credit spread of the counterparty, or the correlation of exposures among the banking organization’s counterparties. Constructing an effective CCR management framework requires a combination of risk management techniques from the credit, market, and operational risk disciplines. </t>
-  </si>
-  <si>
-    <t>Interest rate risk in the banking book is the risk posed by adverse movements in interest rates that cause a mismatch between the rates banks set on customer loans and on deposits.</t>
-  </si>
-  <si>
-    <t>If rates were to increase and a bank’s deposits repriced sooner than its loans, it could result in the bank paying out more interest on deposits than the interest it is receiving from loans. The mismatch would subsequently bite into the bank’s net interest income, as well as affecting the economic value of its equity (EVE), which is derived by discounting future cash inflows and outflows.</t>
-  </si>
-  <si>
-    <t>EVE is specifically used to measure banks’ IRRBB in a standardised outlier test, with supervisors entitled to take action if a bank experiences a change in EVE of more than 15% of common equity Tier 1 under the outlier test.</t>
   </si>
 </sst>
 </file>
@@ -1084,41 +1074,41 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="150.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="150.109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>46</v>
       </c>
@@ -1126,7 +1116,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>48</v>
       </c>
@@ -1134,7 +1124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>50</v>
       </c>
@@ -1142,7 +1132,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
@@ -1159,42 +1149,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E674D334-0D48-4A7D-8DEC-472DB8741757}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="170.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="170.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1210,7 +1200,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1218,7 +1208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
@@ -1226,35 +1216,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
     </row>
   </sheetData>
@@ -1270,33 +1260,33 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="173" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1304,7 +1294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1312,7 +1302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1320,17 +1310,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1338,7 +1328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1346,12 +1336,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1369,42 +1359,42 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="196.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="196.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1422,17 +1412,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="115.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="115.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>56</v>
       </c>
@@ -1450,18 +1440,18 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>72</v>
       </c>
@@ -1469,7 +1459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>74</v>
       </c>
@@ -1477,7 +1467,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>75</v>
       </c>
@@ -1498,70 +1488,70 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="64.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="126.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="64.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="126.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>68</v>
       </c>
@@ -1569,7 +1559,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" ht="72" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
         <v>70</v>
       </c>
@@ -1586,56 +1576,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C6DBE5-F00F-4536-A87D-7667A3F448A1}">
   <dimension ref="B2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="166.5703125" customWidth="1"/>
+    <col min="2" max="2" width="166.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253000A3-156B-4222-8B21-EE119591712E}">
-  <dimension ref="B2:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="175.42578125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>